<commit_message>
ajustes a la carga masiva
</commit_message>
<xml_diff>
--- a/frontend_srp/public/utils/plantilla_estudiantes.xlsx
+++ b/frontend_srp/public/utils/plantilla_estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F366A36F-55B0-4492-A421-3FFE80A9966F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F76A295-296E-4C08-B0BC-A1B89B0E18F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="157">
   <si>
     <t>numero_documento_estudiante</t>
   </si>
@@ -172,9 +172,6 @@
     <t>O Positivo</t>
   </si>
   <si>
-    <t>Padre/Madre</t>
-  </si>
-  <si>
     <t>Ninguna</t>
   </si>
   <si>
@@ -184,69 +181,42 @@
     <t>O Negativo</t>
   </si>
   <si>
-    <t>Tío/Tía</t>
-  </si>
-  <si>
-    <t>Motriz</t>
-  </si>
-  <si>
     <t>A3</t>
   </si>
   <si>
     <t>A Positivo</t>
   </si>
   <si>
-    <t>Abuelo/Abuela</t>
-  </si>
-  <si>
-    <t>Visual</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
     <t>A Negativo</t>
   </si>
   <si>
-    <t>Auditiva</t>
-  </si>
-  <si>
     <t>A5</t>
   </si>
   <si>
     <t>B Positivo</t>
   </si>
   <si>
-    <t>Intelectual</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
     <t>B Negativo</t>
   </si>
   <si>
-    <t>Psicosocial</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
     <t>AB Positivo</t>
   </si>
   <si>
-    <t>Comunicativa</t>
-  </si>
-  <si>
     <t>B3</t>
   </si>
   <si>
     <t>AB Negativo</t>
   </si>
   <si>
-    <t>Múltiple</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
@@ -430,27 +400,12 @@
     <t>Insectos</t>
   </si>
   <si>
-    <t>david</t>
-  </si>
-  <si>
-    <t>d@gmail.com</t>
-  </si>
-  <si>
-    <t>camelia</t>
-  </si>
-  <si>
-    <t>carlos</t>
-  </si>
-  <si>
     <t>fecha_nacimiento(YYYY/MM/DD)</t>
   </si>
   <si>
     <t>id_ciudad</t>
   </si>
   <si>
-    <t>Cedula de extranjeria</t>
-  </si>
-  <si>
     <t>id_genero</t>
   </si>
   <si>
@@ -472,17 +427,92 @@
     <t>id_estado</t>
   </si>
   <si>
-    <t>activo</t>
-  </si>
-  <si>
-    <t>inactivo</t>
+    <t>Procedencia</t>
+  </si>
+  <si>
+    <t>Cédula de extranjería</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>DNI extranjero</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Hermana</t>
+  </si>
+  <si>
+    <t>Hermano</t>
+  </si>
+  <si>
+    <t>Abuela</t>
+  </si>
+  <si>
+    <t>Abuelo</t>
+  </si>
+  <si>
+    <t>Tio</t>
+  </si>
+  <si>
+    <t>Tia</t>
+  </si>
+  <si>
+    <t>Padre</t>
+  </si>
+  <si>
+    <t>Madre</t>
+  </si>
+  <si>
+    <t>Prefiere no decirlo</t>
+  </si>
+  <si>
+    <t>Discapacidad física</t>
+  </si>
+  <si>
+    <t>Discapacidad visual</t>
+  </si>
+  <si>
+    <t>Discapacidad auditiva</t>
+  </si>
+  <si>
+    <t>Discapacidad cognitiva</t>
+  </si>
+  <si>
+    <t>Discapacidad múltiple</t>
+  </si>
+  <si>
+    <t>Discapacidad psicosocial</t>
+  </si>
+  <si>
+    <t>Discapacidad intelectual</t>
+  </si>
+  <si>
+    <t>Discapacidad del habla</t>
+  </si>
+  <si>
+    <t>Movilidad reducida</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Frutos secos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +532,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -560,18 +597,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -629,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{02828455-369D-4E90-A97F-EB8E459D5410}" name="Tabla_acudiente" displayName="Tabla_acudiente" ref="G1:H4" totalsRowShown="0">
-  <autoFilter ref="G1:H4" xr:uid="{02828455-369D-4E90-A97F-EB8E459D5410}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{02828455-369D-4E90-A97F-EB8E459D5410}" name="Tabla_acudiente" displayName="Tabla_acudiente" ref="G1:H10" totalsRowShown="0">
+  <autoFilter ref="G1:H10" xr:uid="{02828455-369D-4E90-A97F-EB8E459D5410}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D1D39AF8-703D-4418-A4C7-961FA1CC970A}" name="id_tipo_acudiente"/>
     <tableColumn id="2" xr3:uid="{C151558E-1F87-46E2-9006-4B3FAAA26FC6}" name="descripcion"/>
@@ -640,8 +672,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{96474B72-501B-4CC5-A37D-B71E1A2EC7B5}" name="Tabla_discapacidad" displayName="Tabla_discapacidad" ref="J1:K9" totalsRowShown="0">
-  <autoFilter ref="J1:K9" xr:uid="{96474B72-501B-4CC5-A37D-B71E1A2EC7B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{96474B72-501B-4CC5-A37D-B71E1A2EC7B5}" name="Tabla_discapacidad" displayName="Tabla_discapacidad" ref="J1:K11" totalsRowShown="0">
+  <autoFilter ref="J1:K11" xr:uid="{96474B72-501B-4CC5-A37D-B71E1A2EC7B5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{EF323230-F09C-45A9-A946-879BF525D876}" name="id_tipo_discapacidad"/>
     <tableColumn id="2" xr3:uid="{058D6B5F-B8FC-4CA7-A49A-90E81F996B1E}" name="descripcion"/>
@@ -651,8 +683,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{29593664-BBB6-41C9-AF69-9366C1327DB4}" name="Tabla_alergia" displayName="Tabla_alergia" ref="M1:N11" totalsRowShown="0">
-  <autoFilter ref="M1:N11" xr:uid="{29593664-BBB6-41C9-AF69-9366C1327DB4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{29593664-BBB6-41C9-AF69-9366C1327DB4}" name="Tabla_alergia" displayName="Tabla_alergia" ref="M1:N12" totalsRowShown="0">
+  <autoFilter ref="M1:N12" xr:uid="{29593664-BBB6-41C9-AF69-9366C1327DB4}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0A703188-A712-4A9B-B235-6DDB1E9F12F9}" name="id_tipo_alergia"/>
     <tableColumn id="2" xr3:uid="{65A90072-7175-4E91-AEEB-76973ED185B4}" name="descripcion"/>
@@ -673,8 +705,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9BFE13F8-D403-4BA7-9063-9C72D389F634}" name="Tabla_documento" displayName="Tabla_documento" ref="S1:T4" totalsRowShown="0">
-  <autoFilter ref="S1:T4" xr:uid="{9BFE13F8-D403-4BA7-9063-9C72D389F634}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9BFE13F8-D403-4BA7-9063-9C72D389F634}" name="Tabla_documento" displayName="Tabla_documento" ref="S1:T6" totalsRowShown="0">
+  <autoFilter ref="S1:T6" xr:uid="{9BFE13F8-D403-4BA7-9063-9C72D389F634}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4BE7FCB5-57C3-49A7-AE91-C9AA24483B23}" name="id_tipo_documento"/>
     <tableColumn id="2" xr3:uid="{EEA862EE-4671-4E9D-A16B-6B25C79D0A34}" name="descripcion"/>
@@ -695,8 +727,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DCBF533F-E64B-47A1-863A-5F3A41E2F590}" name="Tabla_genero" displayName="Tabla_genero" ref="Y1:Z4" totalsRowShown="0">
-  <autoFilter ref="Y1:Z4" xr:uid="{DCBF533F-E64B-47A1-863A-5F3A41E2F590}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DCBF533F-E64B-47A1-863A-5F3A41E2F590}" name="Tabla_genero" displayName="Tabla_genero" ref="Y1:Z6" totalsRowShown="0">
+  <autoFilter ref="Y1:Z6" xr:uid="{DCBF533F-E64B-47A1-863A-5F3A41E2F590}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{75AA66D5-76FE-4D90-BB59-622663803348}" name="id_genero"/>
     <tableColumn id="2" xr3:uid="{686D8FCF-E3E1-4B17-8E8A-6E2151A31DE3}" name="descripcion"/>
@@ -992,29 +1024,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="5" customWidth="1"/>
-    <col min="3" max="6" width="14.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="43" style="5" customWidth="1"/>
-    <col min="11" max="11" width="40.77734375" style="5"/>
-    <col min="12" max="12" width="14.77734375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="18.109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="30.5546875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="22.77734375" style="5" customWidth="1"/>
-    <col min="19" max="19" width="40.77734375" style="5"/>
+    <col min="1" max="1" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="2" customWidth="1"/>
+    <col min="3" max="6" width="14.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="43" style="2" customWidth="1"/>
+    <col min="11" max="11" width="40.77734375" style="2"/>
+    <col min="12" max="12" width="14.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="22.77734375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="29.44140625" style="2" customWidth="1"/>
     <col min="20" max="28" width="40.77734375" style="1"/>
   </cols>
   <sheetData>
@@ -1023,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1047,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>9</v>
@@ -1068,65 +1100,21 @@
         <v>14</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="S1" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>121212</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" s="7">
-        <v>36216</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="P2" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="G2" s="4"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="G3" s="6"/>
+      <c r="G3" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="8">
@@ -1155,24 +1143,21 @@
       <formula1>INDIRECT("Tabla_discapacidad[descripcion]")</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{0C14C242-10CD-4F37-885C-8E60F1C0D9C7}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="67" workbookViewId="0">
+      <selection activeCell="M2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
@@ -1184,7 +1169,7 @@
     <col min="10" max="10" width="24.77734375" style="2" customWidth="1"/>
     <col min="11" max="11" width="39.77734375" style="2" customWidth="1"/>
     <col min="12" max="12" width="27.77734375" style="2" customWidth="1"/>
-    <col min="13" max="23" width="8.88671875" style="1"/>
+    <col min="14" max="23" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
@@ -1223,41 +1208,6 @@
       </c>
       <c r="L1" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1234</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2131213</v>
-      </c>
-      <c r="H2" s="2">
-        <v>213132</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="2">
-        <v>121212</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1280,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,7 +1243,7 @@
     <col min="7" max="7" width="18.109375" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
@@ -1303,7 +1253,7 @@
     <col min="22" max="22" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.33203125" customWidth="1"/>
     <col min="25" max="25" width="11.33203125" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.109375" customWidth="1"/>
     <col min="29" max="29" width="12.44140625" customWidth="1"/>
   </cols>
@@ -1334,37 +1284,37 @@
         <v>39</v>
       </c>
       <c r="M1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="N1" t="s">
         <v>39</v>
       </c>
       <c r="P1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="Q1" t="s">
         <v>39</v>
       </c>
       <c r="S1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="T1" t="s">
         <v>39</v>
       </c>
       <c r="V1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="W1" t="s">
         <v>39</v>
       </c>
       <c r="Y1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="Z1" t="s">
         <v>39</v>
       </c>
       <c r="AB1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="AC1" t="s">
         <v>39</v>
@@ -1387,31 +1337,31 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="V2">
         <v>5001</v>
@@ -1423,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="AB2">
         <v>1</v>
       </c>
       <c r="AC2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -1437,43 +1387,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
       <c r="Q3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="S3">
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="V3">
         <v>5002</v>
@@ -1485,13 +1435,13 @@
         <v>2</v>
       </c>
       <c r="Z3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
       <c r="AC3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
@@ -1499,43 +1449,43 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="P4">
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="V4">
         <v>5003</v>
@@ -1547,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="Z4" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
@@ -1555,37 +1505,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>142</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="P5">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
-        <v>124</v>
+        <v>114</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5" t="s">
+        <v>132</v>
       </c>
       <c r="V5">
         <v>5004</v>
       </c>
       <c r="W5" t="s">
         <v>23</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -1593,31 +1561,51 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>137</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>125</v>
+        <v>115</v>
+      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6" t="s">
+        <v>133</v>
       </c>
       <c r="V6">
         <v>11001</v>
       </c>
       <c r="W6" t="s">
         <v>24</v>
+      </c>
+      <c r="Y6">
+        <v>5</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
@@ -1625,25 +1613,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>138</v>
       </c>
       <c r="J7">
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="V7">
         <v>11002</v>
@@ -1657,25 +1651,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>139</v>
       </c>
       <c r="J8">
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="M8">
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="V8">
         <v>76001</v>
@@ -1689,25 +1689,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>140</v>
       </c>
       <c r="J9">
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="V9">
         <v>76020</v>
@@ -1721,13 +1727,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>153</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="V10">
         <v>76036</v>
@@ -1741,13 +1759,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>154</v>
       </c>
       <c r="M11">
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="V11">
         <v>76068</v>
@@ -1761,7 +1785,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="M12">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>156</v>
       </c>
       <c r="V12">
         <v>76100</v>
@@ -1775,7 +1805,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="V13">
         <v>76109</v>
@@ -1789,7 +1819,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="K14" t="s">
+        <v>155</v>
       </c>
       <c r="V14">
         <v>76122</v>
@@ -1803,7 +1836,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="V15">
         <v>76246</v>
@@ -1817,7 +1850,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="V16">
         <v>76520</v>
@@ -1831,7 +1864,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="V17">
         <v>76736</v>
@@ -1845,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="V18">
         <v>76823</v>
@@ -1859,7 +1892,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="V19">
         <v>76834</v>
@@ -1873,7 +1906,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -1881,7 +1914,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -1889,7 +1922,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -1897,7 +1930,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
@@ -1905,7 +1938,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
@@ -1913,7 +1946,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
@@ -1921,7 +1954,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
@@ -1929,7 +1962,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -1937,7 +1970,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
@@ -1945,7 +1978,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -1953,7 +1986,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -1961,7 +1994,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -1969,7 +2002,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1977,7 +2010,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1985,7 +2018,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1993,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2001,7 +2034,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2009,7 +2042,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2017,7 +2050,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2025,7 +2058,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2033,7 +2066,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2041,7 +2074,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2049,7 +2082,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2057,7 +2090,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2065,7 +2098,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2073,7 +2106,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2114,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2089,7 +2122,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2097,7 +2130,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2105,7 +2138,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2113,7 +2146,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2121,7 +2154,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2129,13 +2162,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="10">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2145,6 +2178,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mas ajustes a la carga masiva
</commit_message>
<xml_diff>
--- a/frontend_srp/public/utils/plantilla_estudiantes.xlsx
+++ b/frontend_srp/public/utils/plantilla_estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F76A295-296E-4C08-B0BC-A1B89B0E18F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956F58A0-33F5-4998-890B-D9370FC6025E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
   <si>
     <t>numero_documento_estudiante</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Bello</t>
   </si>
   <si>
-    <t>Bogotá</t>
-  </si>
-  <si>
     <t>Soacha</t>
   </si>
   <si>
@@ -400,9 +397,6 @@
     <t>Insectos</t>
   </si>
   <si>
-    <t>fecha_nacimiento(YYYY/MM/DD)</t>
-  </si>
-  <si>
     <t>id_ciudad</t>
   </si>
   <si>
@@ -506,12 +500,42 @@
   </si>
   <si>
     <t>Frutos secos</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>d@gmail.com</t>
+  </si>
+  <si>
+    <t>La camelia</t>
+  </si>
+  <si>
+    <t>fecha_nacimiento(YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Catolica</t>
+  </si>
+  <si>
+    <t>emilio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emilio </t>
+  </si>
+  <si>
+    <t>Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>I.E san rafael pombo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,10 +624,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1024,9 +1048,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,11 +1060,11 @@
     <col min="3" max="6" width="14.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="36.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="40.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43" style="2" customWidth="1"/>
     <col min="11" max="11" width="40.77734375" style="2"/>
     <col min="12" max="12" width="14.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="18.109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.44140625" style="2" customWidth="1"/>
@@ -1055,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1079,7 +1103,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>9</v>
@@ -1100,18 +1124,70 @@
         <v>14</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="G2" s="4"/>
-      <c r="J2" s="5"/>
+      <c r="A2" s="2">
+        <v>121212</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="6">
+        <v>40179</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="2">
+        <v>3123212345</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G3" s="4"/>
@@ -1143,16 +1219,19 @@
       <formula1>INDIRECT("Tabla_discapacidad[descripcion]")</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{280F18C0-2C5B-4DEB-AC66-EC4BC20C9CF8}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="M2" sqref="A2:M2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,6 +1289,38 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1234</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3214322123</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2">
+        <v>121212</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{A6A7729A-386D-47EC-AA4C-650DF8926639}">
@@ -1230,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,64 +1371,64 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
-        <v>105</v>
-      </c>
       <c r="T1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="W1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Z1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AC1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
@@ -1325,43 +1436,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V2">
         <v>5001</v>
@@ -1373,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AB2">
         <v>1</v>
       </c>
       <c r="AC2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -1387,43 +1498,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
       <c r="Q3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S3">
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V3">
         <v>5002</v>
@@ -1435,13 +1546,13 @@
         <v>2</v>
       </c>
       <c r="Z3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
       <c r="AC3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
@@ -1449,43 +1560,43 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P4">
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V4">
         <v>5003</v>
@@ -1497,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="Z4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
@@ -1505,43 +1616,43 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P5">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S5">
         <v>4</v>
       </c>
       <c r="T5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V5">
         <v>5004</v>
@@ -1553,7 +1664,7 @@
         <v>4</v>
       </c>
       <c r="Z5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -1561,51 +1672,51 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>115</v>
-      </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
       <c r="S6">
         <v>5</v>
       </c>
       <c r="T6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="V6">
         <v>11001</v>
       </c>
       <c r="W6" t="s">
-        <v>24</v>
+        <v>162</v>
       </c>
       <c r="Y6">
         <v>5</v>
       </c>
       <c r="Z6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
@@ -1613,37 +1724,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J7">
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V7">
         <v>11002</v>
       </c>
       <c r="W7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -1651,37 +1762,37 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J8">
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M8">
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V8">
         <v>76001</v>
       </c>
       <c r="W8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
@@ -1689,37 +1800,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J9">
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V9">
         <v>76020</v>
       </c>
       <c r="W9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -1727,31 +1838,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J10">
         <v>9</v>
       </c>
       <c r="K10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V10">
         <v>76036</v>
       </c>
       <c r="W10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
@@ -1759,25 +1870,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11">
         <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M11">
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V11">
         <v>76068</v>
       </c>
       <c r="W11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
@@ -1785,19 +1896,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12">
         <v>11</v>
       </c>
       <c r="N12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="V12">
         <v>76100</v>
       </c>
       <c r="W12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
@@ -1805,13 +1916,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V13">
         <v>76109</v>
       </c>
       <c r="W13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
@@ -1819,16 +1930,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V14">
         <v>76122</v>
       </c>
       <c r="W14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
@@ -1836,13 +1947,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V15">
         <v>76246</v>
       </c>
       <c r="W15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
@@ -1850,13 +1961,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V16">
         <v>76520</v>
       </c>
       <c r="W16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -1864,13 +1975,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V17">
         <v>76736</v>
       </c>
       <c r="W17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -1878,13 +1989,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V18">
         <v>76823</v>
       </c>
       <c r="W18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -1892,13 +2003,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V19">
         <v>76834</v>
       </c>
       <c r="W19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
@@ -1906,7 +2017,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -1914,7 +2025,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -1922,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -1930,7 +2041,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
@@ -1938,7 +2049,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
@@ -1946,7 +2057,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
@@ -1954,7 +2065,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
@@ -1962,7 +2073,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -1970,7 +2081,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
@@ -1978,7 +2089,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -1986,7 +2097,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -1994,7 +2105,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -2002,7 +2113,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2010,7 +2121,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2018,7 +2129,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2026,7 +2137,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2034,7 +2145,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2042,7 +2153,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2050,7 +2161,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2058,7 +2169,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2066,7 +2177,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2074,7 +2185,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2082,7 +2193,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2090,7 +2201,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2098,7 +2209,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2106,7 +2217,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2114,7 +2225,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2122,7 +2233,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2130,7 +2241,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2138,7 +2249,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2146,7 +2257,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2154,7 +2265,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2162,7 +2273,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>